<commit_message>
Added A1 schematic, Fixed kilometer point units
</commit_message>
<xml_diff>
--- a/data/sensor_locations.xlsx
+++ b/data/sensor_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulinho\Desktop\Master-Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A414B1-6288-40C6-A6C8-2E050DE60E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1CDF8C-6FCC-4E76-947D-7A456C1C806E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD23C080-A3E8-4A95-931E-7578B8E55267}"/>
   </bookViews>
@@ -735,18 +735,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -761,11 +755,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F696A670-22A4-4677-8004-07E2A17F99A5}">
-  <dimension ref="B1:I84"/>
+  <dimension ref="B1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,13 +1101,13 @@
     <col min="2" max="2" width="69.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
     <col min="4" max="4" width="55.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1132,7 +1127,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -1149,7 +1144,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -1166,7 +1161,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -1176,14 +1171,14 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1">
-        <v>1775</v>
+      <c r="E4" s="2">
+        <v>1.7749999999999999</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1200,7 +1195,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -1210,15 +1205,15 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="1">
-        <v>2425</v>
+      <c r="E6" s="2">
+        <v>2.4249999999999998</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -1235,7 +1230,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -1251,9 +1246,9 @@
       <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>33</v>
       </c>
@@ -1269,9 +1264,9 @@
       <c r="F9" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>37</v>
       </c>
@@ -1288,7 +1283,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>42</v>
       </c>
@@ -1304,9 +1299,9 @@
       <c r="F11" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>45</v>
       </c>
@@ -1323,7 +1318,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>48</v>
       </c>
@@ -1340,7 +1335,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>51</v>
       </c>
@@ -1356,8 +1351,9 @@
       <c r="F14" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>52</v>
       </c>
@@ -1374,7 +1370,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>56</v>
       </c>
@@ -1391,7 +1387,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -1407,8 +1403,9 @@
       <c r="F17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>63</v>
       </c>
@@ -1425,7 +1422,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>66</v>
       </c>
@@ -1442,7 +1439,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>70</v>
       </c>
@@ -1459,7 +1456,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>72</v>
       </c>
@@ -1476,7 +1473,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>73</v>
       </c>
@@ -1493,7 +1490,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>76</v>
       </c>
@@ -1503,14 +1500,14 @@
       <c r="D23" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="1">
-        <v>5975</v>
+      <c r="E23" s="2">
+        <v>5.9749999999999996</v>
       </c>
       <c r="F23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>78</v>
       </c>
@@ -1527,7 +1524,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>81</v>
       </c>
@@ -1544,7 +1541,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>84</v>
       </c>
@@ -1554,14 +1551,14 @@
       <c r="D26" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="1">
-        <v>5435</v>
+      <c r="E26" s="2">
+        <v>5.4349999999999996</v>
       </c>
       <c r="F26" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>87</v>
       </c>
@@ -1578,7 +1575,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>90</v>
       </c>
@@ -1595,7 +1592,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>91</v>
       </c>
@@ -1605,14 +1602,14 @@
       <c r="D29" t="s">
         <v>85</v>
       </c>
-      <c r="E29" s="1">
-        <v>5322</v>
+      <c r="E29" s="2">
+        <v>5.3220000000000001</v>
       </c>
       <c r="F29" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>93</v>
       </c>
@@ -1622,14 +1619,14 @@
       <c r="D30" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="1">
-        <v>5322</v>
+      <c r="E30" s="2">
+        <v>5.3220000000000001</v>
       </c>
       <c r="F30" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>94</v>
       </c>
@@ -1639,14 +1636,14 @@
       <c r="D31" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="1">
-        <v>5165</v>
+      <c r="E31" s="2">
+        <v>5.165</v>
       </c>
       <c r="F31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>96</v>
       </c>
@@ -1656,8 +1653,8 @@
       <c r="D32" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="1">
-        <v>5165</v>
+      <c r="E32" s="2">
+        <v>5.165</v>
       </c>
       <c r="F32" t="s">
         <v>95</v>
@@ -1935,7 +1932,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>141</v>
       </c>
@@ -1952,8 +1949,9 @@
         <v>145</v>
       </c>
       <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>146</v>
       </c>
@@ -1970,7 +1968,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>149</v>
       </c>
@@ -1987,7 +1985,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>152</v>
       </c>
@@ -2004,7 +2002,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>153</v>
       </c>
@@ -2014,14 +2012,14 @@
       <c r="D53" t="s">
         <v>85</v>
       </c>
-      <c r="E53" s="1">
-        <v>5435</v>
+      <c r="E53" s="2">
+        <v>5.4349999999999996</v>
       </c>
       <c r="F53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>154</v>
       </c>
@@ -2037,8 +2035,9 @@
       <c r="F54" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>157</v>
       </c>
@@ -2055,7 +2054,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>160</v>
       </c>
@@ -2072,7 +2071,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>163</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>164</v>
       </c>
@@ -2106,7 +2105,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>165</v>
       </c>
@@ -2123,7 +2122,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>166</v>
       </c>
@@ -2140,7 +2139,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>169</v>
       </c>
@@ -2156,8 +2155,9 @@
       <c r="F61" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>173</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>176</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>179</v>
       </c>
@@ -2207,6 +2207,7 @@
       <c r="F64" t="s">
         <v>182</v>
       </c>
+      <c r="H64" s="1"/>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
@@ -2480,7 +2481,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>217</v>
       </c>
@@ -2497,7 +2498,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>218</v>
       </c>
@@ -2513,8 +2514,9 @@
       <c r="F82" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H82" s="4"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>222</v>
       </c>
@@ -2531,7 +2533,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>226</v>
       </c>

</xml_diff>

<commit_message>
Removed Lisbon sensors and Added article data
</commit_message>
<xml_diff>
--- a/data/sensor_locations.xlsx
+++ b/data/sensor_locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulinho\Desktop\Master-Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1CDF8C-6FCC-4E76-947D-7A456C1C806E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3861A23C-F195-4CAF-B69B-77926A9D85FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD23C080-A3E8-4A95-931E-7578B8E55267}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="209">
   <si>
     <t>Equipamento</t>
   </si>
@@ -600,21 +600,6 @@
     <t>AEDL - A20 12+325C PM1214</t>
   </si>
   <si>
-    <t>A1 0+697 C - CAV0101</t>
-  </si>
-  <si>
-    <t>Nó RALIS - Nó IC17/CRIL (Sacavém), sentido descendente</t>
-  </si>
-  <si>
-    <t>0,697</t>
-  </si>
-  <si>
-    <t>(-9.11707 38.7877)</t>
-  </si>
-  <si>
-    <t>A1 0+697 D - CAV0101</t>
-  </si>
-  <si>
     <t>AEDL - A20 6+410C PM1206</t>
   </si>
   <si>
@@ -633,18 +618,6 @@
     <t>(-8.59906 41.1714)</t>
   </si>
   <si>
-    <t>ER108 40+620 (2) Entre-os-Rios (EN108) - Entre-os-Rios (ER108) (22-23) (6637)</t>
-  </si>
-  <si>
-    <t>Nó Carregado - Nó Aveiras de Cima</t>
-  </si>
-  <si>
-    <t>39,95</t>
-  </si>
-  <si>
-    <t>(-8.93356 39.0974)</t>
-  </si>
-  <si>
     <t>ER319 8+700 (2) Monte Cordova - Meixomil (22-15) (6629)</t>
   </si>
   <si>
@@ -654,15 +627,6 @@
     <t>(-8.58092 41.1437)</t>
   </si>
   <si>
-    <t>ER205-4 3+840 (2) Balbeira - Loural (22-06) (6620)</t>
-  </si>
-  <si>
-    <t>Nó IC17/CRIL (Sacavém) - Nó Sta. Iria da Azóia</t>
-  </si>
-  <si>
-    <t>(-9.10192 38.8131)</t>
-  </si>
-  <si>
     <t>AEDL - A1 300+920C PM1209</t>
   </si>
   <si>
@@ -679,30 +643,6 @@
   </si>
   <si>
     <t>AEDL - A20 13+450D PM1215</t>
-  </si>
-  <si>
-    <t>EN349 75+930 (2) Nicho dos Rodrigos - Torres Novas (22-50) (6664)</t>
-  </si>
-  <si>
-    <t>Nó Cartaxo - Nó Santarém</t>
-  </si>
-  <si>
-    <t>58,7</t>
-  </si>
-  <si>
-    <t>(-8.78199 39.2097)</t>
-  </si>
-  <si>
-    <t>ER108 80+520 (2) Baião - São João do Zêzere (22-21) (6635)</t>
-  </si>
-  <si>
-    <t>Nó A1/A15/IP6 - Nó Torres Novas</t>
-  </si>
-  <si>
-    <t>80,5</t>
-  </si>
-  <si>
-    <t>(-8.63459 39.3601)</t>
   </si>
   <si>
     <t>AEDL - A1 297+975C PM1208</t>
@@ -755,11 +695,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -779,8 +717,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:F84" totalsRowShown="0">
-  <autoFilter ref="B1:F84" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:F78" totalsRowShown="0">
+  <autoFilter ref="B1:F78" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{405EBCE7-98B6-4D09-8211-78934C2737E1}" name="Equipamento"/>
     <tableColumn id="2" xr3:uid="{D9489662-8FCF-4FDF-9ADB-D9C7C7021F85}" name="Estrada"/>
@@ -1089,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F696A670-22A4-4677-8004-07E2A17F99A5}">
-  <dimension ref="B1:L84"/>
+  <dimension ref="B1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1062,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
@@ -1171,7 +1109,7 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>1.7749999999999999</v>
       </c>
       <c r="F4" t="s">
@@ -1205,7 +1143,7 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>2.4249999999999998</v>
       </c>
       <c r="F6" t="s">
@@ -1500,7 +1438,7 @@
       <c r="D23" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23">
         <v>5.9749999999999996</v>
       </c>
       <c r="F23" t="s">
@@ -1551,7 +1489,7 @@
       <c r="D26" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
         <v>5.4349999999999996</v>
       </c>
       <c r="F26" t="s">
@@ -1602,7 +1540,7 @@
       <c r="D29" t="s">
         <v>85</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29">
         <v>5.3220000000000001</v>
       </c>
       <c r="F29" t="s">
@@ -1619,7 +1557,7 @@
       <c r="D30" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30">
         <v>5.3220000000000001</v>
       </c>
       <c r="F30" t="s">
@@ -1636,7 +1574,7 @@
       <c r="D31" t="s">
         <v>85</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31">
         <v>5.165</v>
       </c>
       <c r="F31" t="s">
@@ -1653,7 +1591,7 @@
       <c r="D32" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32">
         <v>5.165</v>
       </c>
       <c r="F32" t="s">
@@ -1948,7 +1886,6 @@
       <c r="F49" t="s">
         <v>145</v>
       </c>
-      <c r="G49" s="3"/>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
@@ -2012,7 +1949,7 @@
       <c r="D53" t="s">
         <v>85</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53">
         <v>5.4349999999999996</v>
       </c>
       <c r="F53" t="s">
@@ -2209,7 +2146,7 @@
       </c>
       <c r="H64" s="1"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>183</v>
       </c>
@@ -2225,8 +2162,9 @@
       <c r="F65" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>187</v>
       </c>
@@ -2243,7 +2181,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>189</v>
       </c>
@@ -2260,7 +2198,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>190</v>
       </c>
@@ -2277,278 +2215,181 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>191</v>
       </c>
       <c r="C69" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" t="s">
+        <v>54</v>
+      </c>
+      <c r="F69" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" t="s">
+        <v>194</v>
+      </c>
+      <c r="E70" t="s">
+        <v>195</v>
+      </c>
+      <c r="F70" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>197</v>
+      </c>
+      <c r="C71" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" t="s">
+        <v>198</v>
+      </c>
+      <c r="F71" t="s">
+        <v>199</v>
+      </c>
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>200</v>
+      </c>
+      <c r="C72" t="s">
         <v>142</v>
       </c>
-      <c r="D69" t="s">
-        <v>192</v>
-      </c>
-      <c r="E69" t="s">
-        <v>193</v>
-      </c>
-      <c r="F69" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>195</v>
-      </c>
-      <c r="C70" t="s">
-        <v>142</v>
-      </c>
-      <c r="D70" t="s">
-        <v>192</v>
-      </c>
-      <c r="E70" t="s">
-        <v>193</v>
-      </c>
-      <c r="F70" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>196</v>
-      </c>
-      <c r="C71" t="s">
-        <v>11</v>
-      </c>
-      <c r="D71" t="s">
-        <v>64</v>
-      </c>
-      <c r="E71" t="s">
-        <v>54</v>
-      </c>
-      <c r="F71" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>198</v>
-      </c>
-      <c r="C72" t="s">
-        <v>11</v>
-      </c>
       <c r="D72" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="E72" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="F72" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>202</v>
       </c>
       <c r="C73" t="s">
         <v>142</v>
       </c>
       <c r="D73" t="s">
+        <v>180</v>
+      </c>
+      <c r="E73" t="s">
+        <v>181</v>
+      </c>
+      <c r="F73" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>202</v>
+      </c>
+      <c r="C74" t="s">
+        <v>142</v>
+      </c>
+      <c r="D74" t="s">
+        <v>184</v>
+      </c>
+      <c r="E74" t="s">
+        <v>185</v>
+      </c>
+      <c r="F74" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>203</v>
       </c>
-      <c r="E73" t="s">
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" t="s">
+        <v>121</v>
+      </c>
+      <c r="E75" t="s">
+        <v>122</v>
+      </c>
+      <c r="F75" t="s">
+        <v>123</v>
+      </c>
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
         <v>204</v>
-      </c>
-      <c r="F73" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>206</v>
-      </c>
-      <c r="C74" t="s">
-        <v>11</v>
-      </c>
-      <c r="D74" t="s">
-        <v>12</v>
-      </c>
-      <c r="E74" t="s">
-        <v>207</v>
-      </c>
-      <c r="F74" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>209</v>
-      </c>
-      <c r="C75" t="s">
-        <v>142</v>
-      </c>
-      <c r="D75" t="s">
-        <v>210</v>
-      </c>
-      <c r="E75" t="s">
-        <v>79</v>
-      </c>
-      <c r="F75" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>212</v>
       </c>
       <c r="C76" t="s">
         <v>142</v>
       </c>
       <c r="D76" t="s">
-        <v>180</v>
+        <v>143</v>
       </c>
       <c r="E76" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="F76" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C77" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="D77" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="E77" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="F77" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C78" t="s">
         <v>142</v>
       </c>
       <c r="D78" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="E78" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="F78" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>215</v>
-      </c>
-      <c r="C79" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" t="s">
-        <v>121</v>
-      </c>
-      <c r="E79" t="s">
-        <v>122</v>
-      </c>
-      <c r="F79" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>216</v>
-      </c>
-      <c r="C80" t="s">
-        <v>142</v>
-      </c>
-      <c r="D80" t="s">
-        <v>143</v>
-      </c>
-      <c r="E80" t="s">
-        <v>161</v>
-      </c>
-      <c r="F80" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>217</v>
-      </c>
-      <c r="C81" t="s">
-        <v>11</v>
-      </c>
-      <c r="D81" t="s">
-        <v>114</v>
-      </c>
-      <c r="E81" t="s">
-        <v>155</v>
-      </c>
-      <c r="F81" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>218</v>
-      </c>
-      <c r="C82" t="s">
-        <v>142</v>
-      </c>
-      <c r="D82" t="s">
-        <v>219</v>
-      </c>
-      <c r="E82" t="s">
-        <v>220</v>
-      </c>
-      <c r="F82" t="s">
-        <v>221</v>
-      </c>
-      <c r="H82" s="4"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>222</v>
-      </c>
-      <c r="C83" t="s">
-        <v>142</v>
-      </c>
-      <c r="D83" t="s">
-        <v>223</v>
-      </c>
-      <c r="E83" t="s">
-        <v>224</v>
-      </c>
-      <c r="F83" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>226</v>
-      </c>
-      <c r="C84" t="s">
-        <v>142</v>
-      </c>
-      <c r="D84" t="s">
-        <v>227</v>
-      </c>
-      <c r="E84" t="s">
-        <v>174</v>
-      </c>
-      <c r="F84" t="s">
         <v>175</v>
       </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I81" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Writing node sensors to file
- Removed wrong sensors
- Added first sensor data
</commit_message>
<xml_diff>
--- a/data/sensor_locations.xlsx
+++ b/data/sensor_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulinho\Desktop\Master-Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3861A23C-F195-4CAF-B69B-77926A9D85FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8637615E-CB2E-4318-8034-9DC9726C74D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD23C080-A3E8-4A95-931E-7578B8E55267}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="201">
   <si>
     <t>Equipamento</t>
   </si>
@@ -345,18 +345,6 @@
     <t>(-8.58124 41.153)</t>
   </si>
   <si>
-    <t>A20 8+860D CV726</t>
-  </si>
-  <si>
-    <t>A20 7+965D CV712</t>
-  </si>
-  <si>
-    <t>7,9</t>
-  </si>
-  <si>
-    <t>(-8.5798 41.1371)</t>
-  </si>
-  <si>
     <t>A20 6+410C CV711</t>
   </si>
   <si>
@@ -474,15 +462,6 @@
     <t>(-8.59403 41.1281)</t>
   </si>
   <si>
-    <t>A20 8+860D EM</t>
-  </si>
-  <si>
-    <t>8,8</t>
-  </si>
-  <si>
-    <t>(-8.5809 41.1445)</t>
-  </si>
-  <si>
     <t>A1 300+450C CF</t>
   </si>
   <si>
@@ -634,9 +613,6 @@
   </si>
   <si>
     <t>A1 302+460C CV716</t>
-  </si>
-  <si>
-    <t>AEDL - A44 7+700D PM1205</t>
   </si>
   <si>
     <t>A1 298+680D CV714</t>
@@ -695,10 +671,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,8 +692,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:F78" totalsRowShown="0">
-  <autoFilter ref="B1:F78" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:F74" totalsRowShown="0">
+  <autoFilter ref="B1:F74" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{405EBCE7-98B6-4D09-8211-78934C2737E1}" name="Equipamento"/>
     <tableColumn id="2" xr3:uid="{D9489662-8FCF-4FDF-9ADB-D9C7C7021F85}" name="Estrada"/>
@@ -1027,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F696A670-22A4-4677-8004-07E2A17F99A5}">
-  <dimension ref="B1:L81"/>
+  <dimension ref="B1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,7 +1037,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
@@ -1657,13 +1632,13 @@
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -1674,126 +1649,126 @@
         <v>11</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
         <v>108</v>
-      </c>
-      <c r="F37" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
         <v>110</v>
       </c>
-      <c r="C38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" t="s">
-        <v>64</v>
-      </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="F38" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="E39" t="s">
-        <v>20</v>
+        <v>114</v>
       </c>
       <c r="F39" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E40" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F40" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="E41" t="s">
-        <v>118</v>
+        <v>43</v>
       </c>
       <c r="F41" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E42" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F42" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="E43" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="F43" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="E44" t="s">
         <v>128</v>
@@ -1810,81 +1785,81 @@
         <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="E45" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="F45" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C46" t="s">
         <v>11</v>
       </c>
       <c r="D46" t="s">
-        <v>34</v>
+        <v>134</v>
       </c>
       <c r="E46" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F46" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>67</v>
+        <v>139</v>
       </c>
       <c r="E47" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F47" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="E48" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F48" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>145</v>
+      </c>
+      <c r="C49" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49" t="s">
         <v>141</v>
-      </c>
-      <c r="C49" t="s">
-        <v>142</v>
-      </c>
-      <c r="D49" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" t="s">
-        <v>144</v>
-      </c>
-      <c r="F49" t="s">
-        <v>145</v>
       </c>
       <c r="H49" s="1"/>
     </row>
@@ -1896,47 +1871,47 @@
         <v>6</v>
       </c>
       <c r="D50" t="s">
-        <v>121</v>
-      </c>
-      <c r="E50" t="s">
-        <v>147</v>
+        <v>85</v>
+      </c>
+      <c r="E50">
+        <v>5.4349999999999996</v>
       </c>
       <c r="F50" t="s">
-        <v>148</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
+        <v>147</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" t="s">
+        <v>110</v>
+      </c>
+      <c r="E51" t="s">
+        <v>148</v>
+      </c>
+      <c r="F51" t="s">
         <v>149</v>
-      </c>
-      <c r="C51" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" t="s">
-        <v>150</v>
-      </c>
-      <c r="F51" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
+        <v>150</v>
+      </c>
+      <c r="C52" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" t="s">
+        <v>151</v>
+      </c>
+      <c r="F52" t="s">
         <v>152</v>
-      </c>
-      <c r="C52" t="s">
-        <v>142</v>
-      </c>
-      <c r="D52" t="s">
-        <v>143</v>
-      </c>
-      <c r="E52" t="s">
-        <v>144</v>
-      </c>
-      <c r="F52" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
@@ -1944,33 +1919,33 @@
         <v>153</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
-        <v>85</v>
-      </c>
-      <c r="E53">
-        <v>5.4349999999999996</v>
+        <v>139</v>
+      </c>
+      <c r="E53" t="s">
+        <v>154</v>
       </c>
       <c r="F53" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>156</v>
+      </c>
+      <c r="C54" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" t="s">
         <v>154</v>
       </c>
-      <c r="C54" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" t="s">
-        <v>114</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>155</v>
-      </c>
-      <c r="F54" t="s">
-        <v>156</v>
       </c>
       <c r="K54" s="1"/>
     </row>
@@ -1979,170 +1954,170 @@
         <v>157</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>30</v>
+        <v>139</v>
       </c>
       <c r="E55" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F55" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C56" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E56" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F56" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="D57" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E57" t="s">
+        <v>160</v>
+      </c>
+      <c r="F57" t="s">
         <v>161</v>
-      </c>
-      <c r="F57" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" t="s">
+        <v>163</v>
+      </c>
+      <c r="E58" t="s">
         <v>164</v>
       </c>
-      <c r="C58" t="s">
-        <v>142</v>
-      </c>
-      <c r="D58" t="s">
-        <v>143</v>
-      </c>
-      <c r="E58" t="s">
-        <v>161</v>
-      </c>
       <c r="F58" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C59" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D59" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="E59" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F59" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="D60" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E60" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F60" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C61" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D61" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E61" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F61" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="K61" s="1"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C62" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D62" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E62" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F62" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D63" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="E63" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F63" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>142</v>
+        <v>38</v>
       </c>
       <c r="D64" t="s">
-        <v>180</v>
+        <v>39</v>
       </c>
       <c r="E64" t="s">
-        <v>181</v>
+        <v>43</v>
       </c>
       <c r="F64" t="s">
-        <v>182</v>
+        <v>44</v>
       </c>
       <c r="H64" s="1"/>
     </row>
@@ -2151,51 +2126,51 @@
         <v>183</v>
       </c>
       <c r="C65" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>184</v>
+        <v>34</v>
       </c>
       <c r="E65" t="s">
-        <v>185</v>
+        <v>35</v>
       </c>
       <c r="F65" t="s">
-        <v>186</v>
+        <v>36</v>
       </c>
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C66" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="D66" t="s">
-        <v>184</v>
+        <v>64</v>
       </c>
       <c r="E66" t="s">
+        <v>54</v>
+      </c>
+      <c r="F66" t="s">
         <v>185</v>
-      </c>
-      <c r="F66" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
+        <v>186</v>
+      </c>
+      <c r="C67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" t="s">
+        <v>187</v>
+      </c>
+      <c r="E67" t="s">
+        <v>188</v>
+      </c>
+      <c r="F67" t="s">
         <v>189</v>
-      </c>
-      <c r="C67" t="s">
-        <v>38</v>
-      </c>
-      <c r="D67" t="s">
-        <v>39</v>
-      </c>
-      <c r="E67" t="s">
-        <v>43</v>
-      </c>
-      <c r="F67" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
@@ -2206,190 +2181,123 @@
         <v>11</v>
       </c>
       <c r="D68" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E68" t="s">
-        <v>35</v>
+        <v>191</v>
       </c>
       <c r="F68" t="s">
-        <v>36</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="D69" t="s">
-        <v>64</v>
+        <v>173</v>
       </c>
       <c r="E69" t="s">
-        <v>54</v>
+        <v>174</v>
       </c>
       <c r="F69" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="D70" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="E70" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="F70" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="D71" t="s">
-        <v>12</v>
+        <v>177</v>
       </c>
       <c r="E71" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="F71" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C72" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D72" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="E72" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="F72" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C73" t="s">
-        <v>142</v>
+        <v>11</v>
       </c>
       <c r="D73" t="s">
-        <v>180</v>
+        <v>110</v>
       </c>
       <c r="E73" t="s">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="F73" t="s">
-        <v>182</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C74" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D74" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
       <c r="E74" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="F74" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>203</v>
-      </c>
-      <c r="C75" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" t="s">
-        <v>121</v>
-      </c>
-      <c r="E75" t="s">
-        <v>122</v>
-      </c>
-      <c r="F75" t="s">
-        <v>123</v>
-      </c>
       <c r="H75" s="1"/>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>204</v>
-      </c>
-      <c r="C76" t="s">
-        <v>142</v>
-      </c>
-      <c r="D76" t="s">
-        <v>143</v>
-      </c>
-      <c r="E76" t="s">
-        <v>161</v>
-      </c>
-      <c r="F76" t="s">
-        <v>162</v>
-      </c>
       <c r="I76" s="1"/>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>205</v>
-      </c>
-      <c r="C77" t="s">
-        <v>11</v>
-      </c>
-      <c r="D77" t="s">
-        <v>114</v>
-      </c>
-      <c r="E77" t="s">
-        <v>155</v>
-      </c>
-      <c r="F77" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>206</v>
-      </c>
-      <c r="C78" t="s">
-        <v>142</v>
-      </c>
-      <c r="D78" t="s">
-        <v>207</v>
-      </c>
-      <c r="E78" t="s">
-        <v>174</v>
-      </c>
-      <c r="F78" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I81" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Grouping sensor data into 1-minute blocks
</commit_message>
<xml_diff>
--- a/data/sensor_locations.xlsx
+++ b/data/sensor_locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulinho\Desktop\Master-Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8637615E-CB2E-4318-8034-9DC9726C74D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41404983-11DB-4B42-868A-62D2C32A3D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD23C080-A3E8-4A95-931E-7578B8E55267}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="197">
   <si>
     <t>Equipamento</t>
   </si>
@@ -243,9 +243,6 @@
     <t>(-8.53408 41.1327)</t>
   </si>
   <si>
-    <t>AEDL - A20 6+410D PM1207</t>
-  </si>
-  <si>
     <t>A43 2+416D CV717</t>
   </si>
   <si>
@@ -345,9 +342,6 @@
     <t>(-8.58124 41.153)</t>
   </si>
   <si>
-    <t>A20 6+410C CV711</t>
-  </si>
-  <si>
     <t>A20 3+600D CV710</t>
   </si>
   <si>
@@ -577,12 +571,6 @@
   </si>
   <si>
     <t>AEDL - A20 12+325C PM1214</t>
-  </si>
-  <si>
-    <t>AEDL - A20 6+410C PM1206</t>
-  </si>
-  <si>
-    <t>(-8.57383 41.125)</t>
   </si>
   <si>
     <t>AEDL - A20 12+980 CT3710</t>
@@ -692,8 +680,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:F74" totalsRowShown="0">
-  <autoFilter ref="B1:F74" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:F71" totalsRowShown="0">
+  <autoFilter ref="B1:F71" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{405EBCE7-98B6-4D09-8211-78934C2737E1}" name="Equipamento"/>
     <tableColumn id="2" xr3:uid="{D9489662-8FCF-4FDF-9ADB-D9C7C7021F85}" name="Estrada"/>
@@ -1005,7 +993,7 @@
   <dimension ref="B1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1025,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
@@ -1374,21 +1362,21 @@
         <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
@@ -1396,16 +1384,16 @@
       <c r="D22" t="s">
         <v>39</v>
       </c>
-      <c r="E22" t="s">
-        <v>74</v>
+      <c r="E22">
+        <v>5.9749999999999996</v>
       </c>
       <c r="F22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
@@ -1413,79 +1401,79 @@
       <c r="D23" t="s">
         <v>39</v>
       </c>
-      <c r="E23">
-        <v>5.9749999999999996</v>
+      <c r="E23" t="s">
+        <v>78</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F24" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>53</v>
-      </c>
-      <c r="E25" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="E25">
+        <v>5.4349999999999996</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26">
-        <v>5.4349999999999996</v>
+        <v>84</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" t="s">
         <v>88</v>
-      </c>
-      <c r="F27" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
@@ -1496,30 +1484,30 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+      <c r="E28">
+        <v>5.3220000000000001</v>
       </c>
       <c r="F28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E29">
         <v>5.3220000000000001</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
@@ -1530,30 +1518,30 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E30">
-        <v>5.3220000000000001</v>
+        <v>5.165</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E31">
         <v>5.165</v>
       </c>
       <c r="F31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
@@ -1564,285 +1552,285 @@
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>85</v>
-      </c>
-      <c r="E32">
-        <v>5.165</v>
+        <v>84</v>
+      </c>
+      <c r="E32" t="s">
+        <v>97</v>
       </c>
       <c r="F32" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F34" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="F35" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="F36" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="E37" t="s">
-        <v>20</v>
+        <v>112</v>
       </c>
       <c r="F37" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E38" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="F38" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="E39" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="F39" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F40" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C41" t="s">
         <v>11</v>
       </c>
       <c r="D41" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="E41" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
         <v>11</v>
       </c>
       <c r="D42" t="s">
-        <v>123</v>
+        <v>34</v>
       </c>
       <c r="E42" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F42" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C43" t="s">
         <v>11</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="E43" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="F43" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="E44" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="D45" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="E45" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="F45" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D46" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="E46" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F46" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" t="s">
         <v>137</v>
       </c>
-      <c r="C47" t="s">
+      <c r="E47" t="s">
         <v>138</v>
       </c>
-      <c r="D47" t="s">
+      <c r="F47" t="s">
         <v>139</v>
-      </c>
-      <c r="E47" t="s">
-        <v>140</v>
-      </c>
-      <c r="F47" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48" t="s">
-        <v>117</v>
-      </c>
-      <c r="E48" t="s">
-        <v>143</v>
+        <v>84</v>
+      </c>
+      <c r="E48">
+        <v>5.4349999999999996</v>
       </c>
       <c r="F48" t="s">
-        <v>144</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -1850,85 +1838,85 @@
         <v>145</v>
       </c>
       <c r="C49" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
       <c r="D49" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="E49" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F49" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D50" t="s">
-        <v>85</v>
-      </c>
-      <c r="E50">
-        <v>5.4349999999999996</v>
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>149</v>
       </c>
       <c r="F50" t="s">
-        <v>86</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="D51" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="E51" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F51" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="D52" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
       <c r="E52" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F52" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" t="s">
+        <v>137</v>
+      </c>
+      <c r="E53" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" t="s">
         <v>153</v>
-      </c>
-      <c r="C53" t="s">
-        <v>138</v>
-      </c>
-      <c r="D53" t="s">
-        <v>139</v>
-      </c>
-      <c r="E53" t="s">
-        <v>154</v>
-      </c>
-      <c r="F53" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
@@ -1936,16 +1924,16 @@
         <v>156</v>
       </c>
       <c r="C54" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D54" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E54" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K54" s="1"/>
     </row>
@@ -1954,153 +1942,153 @@
         <v>157</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
       <c r="D55" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E55" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F55" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D56" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="E56" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F56" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="E57" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F57" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D58" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="E58" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F58" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D59" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E59" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="F59" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D60" t="s">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="E60" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="F60" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="C61" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D61" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E61" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F61" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="K61" s="1"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
       <c r="D62" t="s">
-        <v>177</v>
+        <v>39</v>
       </c>
       <c r="E62" t="s">
-        <v>178</v>
+        <v>43</v>
       </c>
       <c r="F62" t="s">
-        <v>179</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C63" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
       <c r="D63" t="s">
-        <v>177</v>
+        <v>34</v>
       </c>
       <c r="E63" t="s">
-        <v>178</v>
+        <v>35</v>
       </c>
       <c r="F63" t="s">
-        <v>181</v>
+        <v>36</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
@@ -2108,190 +2096,139 @@
         <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>39</v>
+        <v>183</v>
       </c>
       <c r="E64" t="s">
-        <v>43</v>
+        <v>184</v>
       </c>
       <c r="F64" t="s">
-        <v>44</v>
+        <v>185</v>
       </c>
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
       </c>
       <c r="D65" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E65" t="s">
-        <v>35</v>
+        <v>187</v>
       </c>
       <c r="F65" t="s">
-        <v>36</v>
+        <v>188</v>
       </c>
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C66" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="D66" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="E66" t="s">
-        <v>54</v>
+        <v>172</v>
       </c>
       <c r="F66" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="D67" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="E67" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="F67" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
-        <v>12</v>
+        <v>175</v>
       </c>
       <c r="E68" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="F68" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C69" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D69" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="E69" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="F69" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C70" t="s">
-        <v>138</v>
+        <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>173</v>
+        <v>108</v>
       </c>
       <c r="E70" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="F70" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
+        <v>194</v>
+      </c>
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+      <c r="D71" t="s">
         <v>195</v>
       </c>
-      <c r="C71" t="s">
-        <v>138</v>
-      </c>
-      <c r="D71" t="s">
-        <v>177</v>
-      </c>
       <c r="E71" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="F71" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="H71" s="1"/>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>196</v>
-      </c>
-      <c r="C72" t="s">
-        <v>138</v>
-      </c>
-      <c r="D72" t="s">
-        <v>139</v>
-      </c>
-      <c r="E72" t="s">
-        <v>154</v>
-      </c>
-      <c r="F72" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>197</v>
-      </c>
-      <c r="C73" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73" t="s">
-        <v>110</v>
-      </c>
-      <c r="E73" t="s">
-        <v>148</v>
-      </c>
-      <c r="F73" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>198</v>
-      </c>
-      <c r="C74" t="s">
-        <v>138</v>
-      </c>
-      <c r="D74" t="s">
-        <v>199</v>
-      </c>
-      <c r="E74" t="s">
-        <v>167</v>
-      </c>
-      <c r="F74" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H75" s="1"/>

</xml_diff>

<commit_message>
Added more sensor data
</commit_message>
<xml_diff>
--- a/data/sensor_locations.xlsx
+++ b/data/sensor_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulinho\Desktop\Master-Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41404983-11DB-4B42-868A-62D2C32A3D65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0EC897-9CD1-444F-A082-4E28DCA459B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD23C080-A3E8-4A95-931E-7578B8E55267}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="181">
   <si>
     <t>Equipamento</t>
   </si>
@@ -57,21 +57,12 @@
     <t>(-8.63107 41.0822)</t>
   </si>
   <si>
-    <t>AEDL - (EP) A20 8+860 CT3706</t>
-  </si>
-  <si>
     <t>A20</t>
   </si>
   <si>
     <t>Nó da Pte. Freixo (S)(A44/IC23) - Nó da Pte. Freixo (N)(N108)</t>
   </si>
   <si>
-    <t>8,86</t>
-  </si>
-  <si>
-    <t>(-8.58106 41.1454)</t>
-  </si>
-  <si>
     <t>CAV403-1/CAV403-2</t>
   </si>
   <si>
@@ -333,15 +324,6 @@
     <t>(-8.61919 41.1222)</t>
   </si>
   <si>
-    <t>A20 9+856C CV727</t>
-  </si>
-  <si>
-    <t>9,8</t>
-  </si>
-  <si>
-    <t>(-8.58124 41.153)</t>
-  </si>
-  <si>
     <t>A20 3+600D CV710</t>
   </si>
   <si>
@@ -402,24 +384,6 @@
     <t>A20 13+890C CV731</t>
   </si>
   <si>
-    <t>A20 12+580C CV729</t>
-  </si>
-  <si>
-    <t>12,5</t>
-  </si>
-  <si>
-    <t>(-8.59428 41.1716)</t>
-  </si>
-  <si>
-    <t>A20 11+700D CV728</t>
-  </si>
-  <si>
-    <t>11,7</t>
-  </si>
-  <si>
-    <t>(-8.58651 41.1671)</t>
-  </si>
-  <si>
     <t>A20 0+575C</t>
   </si>
   <si>
@@ -471,15 +435,6 @@
     <t>(-8.6054 41.1719)</t>
   </si>
   <si>
-    <t>A20 10+970C CV735</t>
-  </si>
-  <si>
-    <t>10,9</t>
-  </si>
-  <si>
-    <t>(-8.58101 41.1625)</t>
-  </si>
-  <si>
     <t>A1 298+680D (Norte)</t>
   </si>
   <si>
@@ -568,9 +523,6 @@
   </si>
   <si>
     <t>A43 2+160</t>
-  </si>
-  <si>
-    <t>AEDL - A20 12+325C PM1214</t>
   </si>
   <si>
     <t>AEDL - A20 12+980 CT3710</t>
@@ -680,8 +632,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:F71" totalsRowShown="0">
-  <autoFilter ref="B1:F71" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:F65" totalsRowShown="0">
+  <autoFilter ref="B1:F65" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{405EBCE7-98B6-4D09-8211-78934C2737E1}" name="Equipamento"/>
     <tableColumn id="2" xr3:uid="{D9489662-8FCF-4FDF-9ADB-D9C7C7021F85}" name="Estrada"/>
@@ -993,7 +945,7 @@
   <dimension ref="B1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,7 +977,7 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
@@ -1047,16 +999,16 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
         <v>13</v>
+      </c>
+      <c r="E3">
+        <v>1.7749999999999999</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -1072,25 +1024,25 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
-        <v>1.7749999999999999</v>
+      <c r="E4" t="s">
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
         <v>20</v>
+      </c>
+      <c r="E5">
+        <v>2.4249999999999998</v>
       </c>
       <c r="F5" t="s">
         <v>21</v>
@@ -1101,81 +1053,81 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6">
-        <v>2.4249999999999998</v>
+      <c r="E6" t="s">
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
         <v>40</v>
@@ -1189,10 +1141,10 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
         <v>43</v>
@@ -1207,10 +1159,10 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
         <v>46</v>
@@ -1224,62 +1176,62 @@
         <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
         <v>51</v>
       </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>49</v>
-      </c>
       <c r="F14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
         <v>58</v>
@@ -1293,13 +1245,13 @@
         <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
         <v>62</v>
@@ -1311,47 +1263,47 @@
         <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D18" t="s">
         <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
         <v>68</v>
-      </c>
-      <c r="F19" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
         <v>70</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>54</v>
       </c>
       <c r="F20" t="s">
         <v>71</v>
@@ -1362,30 +1314,30 @@
         <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>5.9749999999999996</v>
+      </c>
+      <c r="F21" t="s">
         <v>73</v>
-      </c>
-      <c r="F21" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
         <v>75</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22">
-        <v>5.9749999999999996</v>
       </c>
       <c r="F22" t="s">
         <v>76</v>
@@ -1396,10 +1348,10 @@
         <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
         <v>78</v>
@@ -1416,10 +1368,10 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" t="s">
         <v>81</v>
+      </c>
+      <c r="E24">
+        <v>5.4349999999999996</v>
       </c>
       <c r="F24" t="s">
         <v>82</v>
@@ -1433,10 +1385,10 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" t="s">
         <v>84</v>
-      </c>
-      <c r="E25">
-        <v>5.4349999999999996</v>
       </c>
       <c r="F25" t="s">
         <v>85</v>
@@ -1450,27 +1402,27 @@
         <v>6</v>
       </c>
       <c r="D26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" t="s">
         <v>84</v>
       </c>
-      <c r="E26" t="s">
-        <v>87</v>
-      </c>
       <c r="F26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="E27">
+        <v>5.3220000000000001</v>
       </c>
       <c r="F27" t="s">
         <v>88</v>
@@ -1478,33 +1430,33 @@
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E28">
         <v>5.3220000000000001</v>
       </c>
       <c r="F28" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E29">
-        <v>5.3220000000000001</v>
+        <v>5.165</v>
       </c>
       <c r="F29" t="s">
         <v>91</v>
@@ -1512,36 +1464,36 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E30">
         <v>5.165</v>
       </c>
       <c r="F30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
-      </c>
-      <c r="E31">
-        <v>5.165</v>
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
       </c>
       <c r="F31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
@@ -1552,7 +1504,7 @@
         <v>6</v>
       </c>
       <c r="D32" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
         <v>97</v>
@@ -1566,27 +1518,27 @@
         <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" t="s">
         <v>100</v>
-      </c>
-      <c r="F33" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
         <v>102</v>
-      </c>
-      <c r="C34" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" t="s">
-        <v>30</v>
       </c>
       <c r="E34" t="s">
         <v>103</v>
@@ -1600,47 +1552,47 @@
         <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="F35" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D36" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E36" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F36" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>40</v>
       </c>
       <c r="F37" t="s">
         <v>113</v>
@@ -1651,7 +1603,7 @@
         <v>114</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D38" t="s">
         <v>115</v>
@@ -1668,335 +1620,335 @@
         <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D39" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="F39" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" t="s">
         <v>120</v>
       </c>
-      <c r="C40" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>121</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>122</v>
-      </c>
-      <c r="F40" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" t="s">
         <v>124</v>
       </c>
-      <c r="C41" t="s">
-        <v>11</v>
-      </c>
       <c r="D41" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="E41" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="F41" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D42" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="F42" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="E43" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F43" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D44" t="s">
-        <v>132</v>
-      </c>
-      <c r="E44" t="s">
-        <v>133</v>
+        <v>81</v>
+      </c>
+      <c r="E44">
+        <v>5.4349999999999996</v>
       </c>
       <c r="F44" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" t="s">
+        <v>134</v>
+      </c>
+      <c r="F45" t="s">
         <v>135</v>
-      </c>
-      <c r="C45" t="s">
-        <v>136</v>
-      </c>
-      <c r="D45" t="s">
-        <v>137</v>
-      </c>
-      <c r="E45" t="s">
-        <v>138</v>
-      </c>
-      <c r="F45" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="D46" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E46" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F46" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C47" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D47" t="s">
+        <v>125</v>
+      </c>
+      <c r="E47" t="s">
         <v>137</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>138</v>
-      </c>
-      <c r="F47" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="D48" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48">
-        <v>5.4349999999999996</v>
+        <v>125</v>
+      </c>
+      <c r="E48" t="s">
+        <v>137</v>
       </c>
       <c r="F48" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="D49" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F49" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="E50" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F50" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C51" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E51" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F51" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="E52" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F52" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C53" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E53" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F53" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" t="s">
+        <v>124</v>
+      </c>
+      <c r="D54" t="s">
         <v>156</v>
       </c>
-      <c r="C54" t="s">
-        <v>136</v>
-      </c>
-      <c r="D54" t="s">
-        <v>137</v>
-      </c>
       <c r="E54" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="F54" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="D55" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="E55" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F55" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
+        <v>163</v>
+      </c>
+      <c r="C56" t="s">
+        <v>124</v>
+      </c>
+      <c r="D56" t="s">
         <v>160</v>
       </c>
-      <c r="C56" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>161</v>
       </c>
-      <c r="E56" t="s">
-        <v>162</v>
-      </c>
       <c r="F56" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>35</v>
       </c>
       <c r="D57" t="s">
-        <v>161</v>
+        <v>36</v>
       </c>
       <c r="E57" t="s">
-        <v>165</v>
+        <v>40</v>
       </c>
       <c r="F57" t="s">
-        <v>166</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" t="s">
         <v>167</v>
-      </c>
-      <c r="C58" t="s">
-        <v>136</v>
-      </c>
-      <c r="D58" t="s">
-        <v>137</v>
       </c>
       <c r="E58" t="s">
         <v>168</v>
@@ -2010,224 +1962,124 @@
         <v>170</v>
       </c>
       <c r="C59" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="D59" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
         <v>171</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>172</v>
-      </c>
-      <c r="F59" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C60" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D60" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E60" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="F60" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C61" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D61" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E61" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="F61" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="K61" s="1"/>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="D62" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
       <c r="E62" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="F62" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="D63" t="s">
-        <v>34</v>
+        <v>125</v>
       </c>
       <c r="E63" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="F63" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>183</v>
+        <v>102</v>
       </c>
       <c r="E64" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="F64" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="D65" t="s">
-        <v>12</v>
+        <v>179</v>
       </c>
       <c r="E65" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="F65" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>189</v>
-      </c>
-      <c r="C66" t="s">
-        <v>136</v>
-      </c>
-      <c r="D66" t="s">
-        <v>171</v>
-      </c>
-      <c r="E66" t="s">
-        <v>172</v>
-      </c>
-      <c r="F66" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>190</v>
-      </c>
-      <c r="C67" t="s">
-        <v>136</v>
-      </c>
-      <c r="D67" t="s">
-        <v>171</v>
-      </c>
-      <c r="E67" t="s">
-        <v>172</v>
-      </c>
-      <c r="F67" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>191</v>
-      </c>
-      <c r="C68" t="s">
-        <v>136</v>
-      </c>
-      <c r="D68" t="s">
-        <v>175</v>
-      </c>
-      <c r="E68" t="s">
-        <v>176</v>
-      </c>
-      <c r="F68" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>192</v>
-      </c>
-      <c r="C69" t="s">
-        <v>136</v>
-      </c>
-      <c r="D69" t="s">
-        <v>137</v>
-      </c>
-      <c r="E69" t="s">
-        <v>152</v>
-      </c>
-      <c r="F69" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>193</v>
-      </c>
-      <c r="C70" t="s">
-        <v>11</v>
-      </c>
-      <c r="D70" t="s">
-        <v>108</v>
-      </c>
-      <c r="E70" t="s">
-        <v>146</v>
-      </c>
-      <c r="F70" t="s">
-        <v>147</v>
-      </c>
-    </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>194</v>
-      </c>
-      <c r="C71" t="s">
-        <v>136</v>
-      </c>
-      <c r="D71" t="s">
-        <v>195</v>
-      </c>
-      <c r="E71" t="s">
-        <v>165</v>
-      </c>
-      <c r="F71" t="s">
-        <v>166</v>
-      </c>
       <c r="H71" s="1"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Processing multiple data sheets of sensors
</commit_message>
<xml_diff>
--- a/data/sensor_locations.xlsx
+++ b/data/sensor_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulinho\Desktop\Master-Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CDF39F-A4ED-4130-B301-A42731D06367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFE9E16-B619-404E-93E0-93735E8C7E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD23C080-A3E8-4A95-931E-7578B8E55267}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="203">
   <si>
     <t>Equipamento</t>
   </si>
@@ -369,21 +369,6 @@
     <t>(-8.57493 41.0906)</t>
   </si>
   <si>
-    <t>A20 14+980C CV732</t>
-  </si>
-  <si>
-    <t>Amial - N14/Circunvalação</t>
-  </si>
-  <si>
-    <t>14,9</t>
-  </si>
-  <si>
-    <t>(-8.62146 41.1735)</t>
-  </si>
-  <si>
-    <t>A20 13+890C CV731</t>
-  </si>
-  <si>
     <t>A20 0+575C</t>
   </si>
   <si>
@@ -426,15 +411,6 @@
     <t>A44 5+435D CVT741</t>
   </si>
   <si>
-    <t>A20 13+450D CV730</t>
-  </si>
-  <si>
-    <t>13,4</t>
-  </si>
-  <si>
-    <t>(-8.6054 41.1719)</t>
-  </si>
-  <si>
     <t>A1 298+680D (Norte)</t>
   </si>
   <si>
@@ -556,9 +532,6 @@
   </si>
   <si>
     <t>A1 298+680D CV714</t>
-  </si>
-  <si>
-    <t>AEDL - A20 13+450D PM1215</t>
   </si>
   <si>
     <t>AEDL - A1 297+975C PM1208</t>
@@ -704,10 +677,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,8 +698,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:G79" totalsRowShown="0">
-  <autoFilter ref="B1:G79" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:G75" totalsRowShown="0">
+  <autoFilter ref="B1:G75" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{DA4E266E-78B3-49ED-9193-E0A12C370FEF}" name="Network"/>
     <tableColumn id="1" xr3:uid="{405EBCE7-98B6-4D09-8211-78934C2737E1}" name="Equipamento"/>
@@ -1037,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F696A670-22A4-4677-8004-07E2A17F99A5}">
-  <dimension ref="B1:M82"/>
+  <dimension ref="B1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1029,7 @@
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1075,12 +1047,12 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>210</v>
+      <c r="B2" t="s">
+        <v>201</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1099,8 +1071,8 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>210</v>
+      <c r="B3" t="s">
+        <v>201</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1119,8 +1091,8 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>210</v>
+      <c r="B4" t="s">
+        <v>201</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -1139,8 +1111,8 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>210</v>
+      <c r="B5" t="s">
+        <v>201</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -1159,8 +1131,8 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>210</v>
+      <c r="B6" t="s">
+        <v>201</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -1180,8 +1152,8 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>210</v>
+      <c r="B7" t="s">
+        <v>201</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -1200,8 +1172,8 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>210</v>
+      <c r="B8" t="s">
+        <v>201</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -1221,8 +1193,8 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>210</v>
+      <c r="B9" t="s">
+        <v>201</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -1242,8 +1214,8 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>210</v>
+      <c r="B10" t="s">
+        <v>201</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1262,8 +1234,8 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>210</v>
+      <c r="B11" t="s">
+        <v>201</v>
       </c>
       <c r="C11" t="s">
         <v>42</v>
@@ -1283,8 +1255,8 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>210</v>
+      <c r="B12" t="s">
+        <v>201</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
@@ -1303,8 +1275,8 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>210</v>
+      <c r="B13" t="s">
+        <v>201</v>
       </c>
       <c r="C13" t="s">
         <v>48</v>
@@ -1323,8 +1295,8 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>210</v>
+      <c r="B14" t="s">
+        <v>201</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
@@ -1344,8 +1316,8 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>210</v>
+      <c r="B15" t="s">
+        <v>201</v>
       </c>
       <c r="C15" t="s">
         <v>53</v>
@@ -1364,8 +1336,8 @@
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>210</v>
+      <c r="B16" t="s">
+        <v>201</v>
       </c>
       <c r="C16" t="s">
         <v>57</v>
@@ -1384,8 +1356,8 @@
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>210</v>
+      <c r="B17" t="s">
+        <v>201</v>
       </c>
       <c r="C17" t="s">
         <v>60</v>
@@ -1405,8 +1377,8 @@
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>210</v>
+      <c r="B18" t="s">
+        <v>201</v>
       </c>
       <c r="C18" t="s">
         <v>63</v>
@@ -1425,8 +1397,8 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>210</v>
+      <c r="B19" t="s">
+        <v>201</v>
       </c>
       <c r="C19" t="s">
         <v>67</v>
@@ -1445,8 +1417,8 @@
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>210</v>
+      <c r="B20" t="s">
+        <v>201</v>
       </c>
       <c r="C20" t="s">
         <v>69</v>
@@ -1465,8 +1437,8 @@
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>210</v>
+      <c r="B21" t="s">
+        <v>201</v>
       </c>
       <c r="C21" t="s">
         <v>72</v>
@@ -1485,8 +1457,8 @@
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>210</v>
+      <c r="B22" t="s">
+        <v>201</v>
       </c>
       <c r="C22" t="s">
         <v>74</v>
@@ -1505,8 +1477,8 @@
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>210</v>
+      <c r="B23" t="s">
+        <v>201</v>
       </c>
       <c r="C23" t="s">
         <v>77</v>
@@ -1525,8 +1497,8 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>210</v>
+      <c r="B24" t="s">
+        <v>201</v>
       </c>
       <c r="C24" t="s">
         <v>80</v>
@@ -1545,8 +1517,8 @@
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>210</v>
+      <c r="B25" t="s">
+        <v>201</v>
       </c>
       <c r="C25" t="s">
         <v>83</v>
@@ -1565,8 +1537,8 @@
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>210</v>
+      <c r="B26" t="s">
+        <v>201</v>
       </c>
       <c r="C26" t="s">
         <v>86</v>
@@ -1585,8 +1557,8 @@
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>210</v>
+      <c r="B27" t="s">
+        <v>201</v>
       </c>
       <c r="C27" t="s">
         <v>87</v>
@@ -1605,8 +1577,8 @@
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>210</v>
+      <c r="B28" t="s">
+        <v>201</v>
       </c>
       <c r="C28" t="s">
         <v>89</v>
@@ -1625,8 +1597,8 @@
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>210</v>
+      <c r="B29" t="s">
+        <v>201</v>
       </c>
       <c r="C29" t="s">
         <v>90</v>
@@ -1645,8 +1617,8 @@
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>210</v>
+      <c r="B30" t="s">
+        <v>201</v>
       </c>
       <c r="C30" t="s">
         <v>92</v>
@@ -1665,8 +1637,8 @@
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>210</v>
+      <c r="B31" t="s">
+        <v>201</v>
       </c>
       <c r="C31" t="s">
         <v>93</v>
@@ -1685,8 +1657,8 @@
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>210</v>
+      <c r="B32" t="s">
+        <v>201</v>
       </c>
       <c r="C32" t="s">
         <v>96</v>
@@ -1705,8 +1677,8 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="2" t="s">
-        <v>210</v>
+      <c r="B33" t="s">
+        <v>201</v>
       </c>
       <c r="C33" t="s">
         <v>99</v>
@@ -1725,8 +1697,8 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>210</v>
+      <c r="B34" t="s">
+        <v>201</v>
       </c>
       <c r="C34" t="s">
         <v>101</v>
@@ -1745,8 +1717,8 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>210</v>
+      <c r="B35" t="s">
+        <v>201</v>
       </c>
       <c r="C35" t="s">
         <v>105</v>
@@ -1765,8 +1737,8 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>210</v>
+      <c r="B36" t="s">
+        <v>201</v>
       </c>
       <c r="C36" t="s">
         <v>108</v>
@@ -1785,8 +1757,8 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>210</v>
+      <c r="B37" t="s">
+        <v>201</v>
       </c>
       <c r="C37" t="s">
         <v>112</v>
@@ -1805,8 +1777,8 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>210</v>
+      <c r="B38" t="s">
+        <v>201</v>
       </c>
       <c r="C38" t="s">
         <v>114</v>
@@ -1825,709 +1797,628 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
-        <v>210</v>
+      <c r="B39" t="s">
+        <v>201</v>
       </c>
       <c r="C39" t="s">
         <v>118</v>
       </c>
       <c r="D39" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="E39" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="F39" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="G39" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>210</v>
+      <c r="B40" t="s">
+        <v>201</v>
       </c>
       <c r="C40" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>109</v>
+      </c>
+      <c r="F40" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" t="s">
         <v>119</v>
       </c>
-      <c r="D40" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>120</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>121</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G41" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C41" t="s">
-        <v>123</v>
-      </c>
-      <c r="D41" t="s">
-        <v>124</v>
-      </c>
-      <c r="E41" t="s">
-        <v>125</v>
-      </c>
-      <c r="F41" t="s">
-        <v>126</v>
-      </c>
-      <c r="G41" t="s">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C42" t="s">
-        <v>128</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>109</v>
-      </c>
-      <c r="F42" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42">
+        <v>5.4349999999999996</v>
+      </c>
+      <c r="G42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>201</v>
+      </c>
+      <c r="C43" t="s">
+        <v>128</v>
+      </c>
+      <c r="D43" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" t="s">
+        <v>120</v>
+      </c>
+      <c r="F43" t="s">
         <v>129</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G43" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C43" t="s">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>201</v>
+      </c>
+      <c r="C44" t="s">
         <v>131</v>
       </c>
-      <c r="D43" t="s">
-        <v>124</v>
-      </c>
-      <c r="E43" t="s">
-        <v>125</v>
-      </c>
-      <c r="F43" t="s">
-        <v>126</v>
-      </c>
-      <c r="G43" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" t="s">
         <v>132</v>
       </c>
-      <c r="D44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" t="s">
-        <v>81</v>
-      </c>
-      <c r="F44">
-        <v>5.4349999999999996</v>
-      </c>
-      <c r="G44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" t="s">
+        <v>120</v>
+      </c>
+      <c r="F45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>201</v>
+      </c>
+      <c r="C46" t="s">
         <v>133</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" t="s">
+        <v>120</v>
+      </c>
+      <c r="F46" t="s">
+        <v>129</v>
+      </c>
+      <c r="G46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" t="s">
         <v>10</v>
       </c>
-      <c r="E45" t="s">
-        <v>102</v>
-      </c>
-      <c r="F45" t="s">
-        <v>134</v>
-      </c>
-      <c r="G45" t="s">
+      <c r="E47" t="s">
+        <v>115</v>
+      </c>
+      <c r="F47" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="G47" t="s">
         <v>136</v>
       </c>
-      <c r="D46" t="s">
-        <v>124</v>
-      </c>
-      <c r="E46" t="s">
-        <v>125</v>
-      </c>
-      <c r="F46" t="s">
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>201</v>
+      </c>
+      <c r="C48" t="s">
         <v>137</v>
       </c>
-      <c r="G46" t="s">
+      <c r="D48" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="F48" t="s">
         <v>139</v>
       </c>
-      <c r="D47" t="s">
-        <v>124</v>
-      </c>
-      <c r="E47" t="s">
-        <v>125</v>
-      </c>
-      <c r="F47" t="s">
-        <v>137</v>
-      </c>
-      <c r="G47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="G48" t="s">
         <v>140</v>
       </c>
-      <c r="D48" t="s">
-        <v>124</v>
-      </c>
-      <c r="E48" t="s">
-        <v>125</v>
-      </c>
-      <c r="F48" t="s">
-        <v>137</v>
-      </c>
-      <c r="G48" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>210</v>
+      <c r="B49" t="s">
+        <v>201</v>
       </c>
       <c r="C49" t="s">
         <v>141</v>
       </c>
       <c r="D49" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E49" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="F49" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="G49" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
-        <v>210</v>
+      <c r="B50" t="s">
+        <v>201</v>
       </c>
       <c r="C50" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D50" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="E50" t="s">
         <v>120</v>
       </c>
       <c r="F50" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G50" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
-        <v>210</v>
+      <c r="B51" t="s">
+        <v>201</v>
       </c>
       <c r="C51" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D51" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E51" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F51" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G51" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>210</v>
+      <c r="B52" t="s">
+        <v>201</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D52" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E52" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F52" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G52" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>210</v>
+      <c r="B53" t="s">
+        <v>201</v>
       </c>
       <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="D53" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53" t="s">
         <v>152</v>
-      </c>
-      <c r="D53" t="s">
-        <v>124</v>
-      </c>
-      <c r="E53" t="s">
-        <v>125</v>
       </c>
       <c r="F53" t="s">
         <v>153</v>
       </c>
       <c r="G53" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" s="2" t="s">
-        <v>210</v>
+      <c r="B54" t="s">
+        <v>201</v>
       </c>
       <c r="C54" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D54" t="s">
-        <v>124</v>
+        <v>35</v>
       </c>
       <c r="E54" t="s">
-        <v>156</v>
+        <v>36</v>
       </c>
       <c r="F54" t="s">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="G54" t="s">
+        <v>41</v>
+      </c>
+      <c r="L54" s="1"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>201</v>
+      </c>
+      <c r="C55" t="s">
         <v>158</v>
       </c>
-      <c r="L54" s="1"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" t="s">
         <v>159</v>
       </c>
-      <c r="D55" t="s">
-        <v>124</v>
-      </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>160</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>161</v>
       </c>
-      <c r="G55" t="s">
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>201</v>
+      </c>
+      <c r="C56" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" t="s">
         <v>163</v>
-      </c>
-      <c r="D56" t="s">
-        <v>124</v>
-      </c>
-      <c r="E56" t="s">
-        <v>160</v>
-      </c>
-      <c r="F56" t="s">
-        <v>161</v>
       </c>
       <c r="G56" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
-        <v>210</v>
+      <c r="B57" t="s">
+        <v>201</v>
       </c>
       <c r="C57" t="s">
         <v>165</v>
       </c>
       <c r="D57" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="E57" t="s">
-        <v>36</v>
+        <v>148</v>
       </c>
       <c r="F57" t="s">
-        <v>40</v>
+        <v>149</v>
       </c>
       <c r="G57" t="s">
-        <v>41</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
-        <v>210</v>
+      <c r="B58" t="s">
+        <v>201</v>
       </c>
       <c r="C58" t="s">
         <v>166</v>
       </c>
       <c r="D58" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="E58" t="s">
+        <v>148</v>
+      </c>
+      <c r="F58" t="s">
+        <v>149</v>
+      </c>
+      <c r="G58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>201</v>
+      </c>
+      <c r="C59" t="s">
         <v>167</v>
       </c>
-      <c r="F58" t="s">
+      <c r="D59" t="s">
+        <v>119</v>
+      </c>
+      <c r="E59" t="s">
+        <v>152</v>
+      </c>
+      <c r="F59" t="s">
+        <v>153</v>
+      </c>
+      <c r="G59" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>201</v>
+      </c>
+      <c r="C60" t="s">
         <v>168</v>
       </c>
-      <c r="G58" t="s">
+      <c r="D60" t="s">
+        <v>119</v>
+      </c>
+      <c r="E60" t="s">
+        <v>120</v>
+      </c>
+      <c r="F60" t="s">
+        <v>129</v>
+      </c>
+      <c r="G60" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>201</v>
+      </c>
+      <c r="C61" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D61" t="s">
+        <v>119</v>
+      </c>
+      <c r="E61" t="s">
         <v>170</v>
       </c>
-      <c r="D59" t="s">
-        <v>10</v>
-      </c>
-      <c r="E59" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" t="s">
-        <v>171</v>
-      </c>
-      <c r="G59" t="s">
+      <c r="F61" t="s">
+        <v>142</v>
+      </c>
+      <c r="G61" t="s">
+        <v>143</v>
+      </c>
+      <c r="L61" s="1"/>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>202</v>
+      </c>
+      <c r="C62" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B60" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="G62" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>202</v>
+      </c>
+      <c r="C63" t="s">
         <v>173</v>
       </c>
-      <c r="D60" t="s">
-        <v>124</v>
-      </c>
-      <c r="E60" t="s">
-        <v>156</v>
-      </c>
-      <c r="F60" t="s">
-        <v>157</v>
-      </c>
-      <c r="G60" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B61" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="G63" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>202</v>
+      </c>
+      <c r="C64" t="s">
         <v>174</v>
       </c>
-      <c r="D61" t="s">
-        <v>124</v>
-      </c>
-      <c r="E61" t="s">
-        <v>156</v>
-      </c>
-      <c r="F61" t="s">
-        <v>157</v>
-      </c>
-      <c r="G61" t="s">
-        <v>158</v>
-      </c>
-      <c r="L61" s="1"/>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="G64" t="s">
+        <v>178</v>
+      </c>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>202</v>
+      </c>
+      <c r="C65" t="s">
         <v>175</v>
       </c>
-      <c r="D62" t="s">
-        <v>124</v>
-      </c>
-      <c r="E62" t="s">
-        <v>160</v>
-      </c>
-      <c r="F62" t="s">
-        <v>161</v>
-      </c>
-      <c r="G62" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B63" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C63" t="s">
-        <v>176</v>
-      </c>
-      <c r="D63" t="s">
-        <v>124</v>
-      </c>
-      <c r="E63" t="s">
-        <v>125</v>
-      </c>
-      <c r="F63" t="s">
-        <v>137</v>
-      </c>
-      <c r="G63" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B64" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C64" t="s">
-        <v>177</v>
-      </c>
-      <c r="D64" t="s">
-        <v>10</v>
-      </c>
-      <c r="E64" t="s">
-        <v>102</v>
-      </c>
-      <c r="F64" t="s">
-        <v>134</v>
-      </c>
-      <c r="G64" t="s">
-        <v>135</v>
-      </c>
-      <c r="I64" s="1"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C65" t="s">
-        <v>178</v>
-      </c>
-      <c r="D65" t="s">
-        <v>124</v>
-      </c>
-      <c r="E65" t="s">
+      <c r="G65" t="s">
         <v>179</v>
-      </c>
-      <c r="F65" t="s">
-        <v>150</v>
-      </c>
-      <c r="G65" t="s">
-        <v>151</v>
       </c>
       <c r="I65" s="1"/>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C66" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G66" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C67" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G67" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C68" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G68" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C69" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G70" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C71" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G71" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I71" s="1"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C72" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G72" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C73" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G73" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C74" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="G74" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C75" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G75" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I75" s="1"/>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>211</v>
-      </c>
-      <c r="C76" t="s">
-        <v>199</v>
-      </c>
-      <c r="G76" t="s">
-        <v>205</v>
-      </c>
       <c r="J76" s="1"/>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>211</v>
-      </c>
-      <c r="C77" t="s">
-        <v>200</v>
-      </c>
-      <c r="G77" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>211</v>
-      </c>
-      <c r="C78" t="s">
-        <v>201</v>
-      </c>
-      <c r="G78" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>211</v>
-      </c>
-      <c r="C79" t="s">
-        <v>202</v>
-      </c>
-      <c r="G79" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added new sensor data
</commit_message>
<xml_diff>
--- a/data/sensor_locations.xlsx
+++ b/data/sensor_locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulinho\Desktop\Master-Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFE9E16-B619-404E-93E0-93735E8C7E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8D14DE-85DD-49AB-BB51-B3B8FC8D734E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD23C080-A3E8-4A95-931E-7578B8E55267}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="143">
   <si>
     <t>Equipamento</t>
   </si>
@@ -171,9 +171,6 @@
     <t>(-8.55682 41.1552)</t>
   </si>
   <si>
-    <t>AEDL - A43 3+100D PM1211</t>
-  </si>
-  <si>
     <t>AEDL - A44 6+425 CT3681</t>
   </si>
   <si>
@@ -234,102 +231,9 @@
     <t>(-8.53408 41.1327)</t>
   </si>
   <si>
-    <t>A43 2+416D CV717</t>
-  </si>
-  <si>
-    <t>2,4</t>
-  </si>
-  <si>
-    <t>(-8.56314 41.1584)</t>
-  </si>
-  <si>
-    <t>A43 5+975C CV719</t>
-  </si>
-  <si>
-    <t>(-8.53695 41.1354)</t>
-  </si>
-  <si>
-    <t>A43 3+840D CV718</t>
-  </si>
-  <si>
-    <t>3,8</t>
-  </si>
-  <si>
-    <t>(-8.5494 41.1523)</t>
-  </si>
-  <si>
-    <t>A44 5+750C CV748</t>
-  </si>
-  <si>
-    <t>5,75</t>
-  </si>
-  <si>
-    <t>(-8.60887 41.1247)</t>
-  </si>
-  <si>
-    <t>A44 5+435C CVT742</t>
-  </si>
-  <si>
     <t>Coimbrões - Av. Da República</t>
   </si>
   <si>
-    <t>(-8.61222 41.1235)</t>
-  </si>
-  <si>
-    <t>A44 5+380D CVT745</t>
-  </si>
-  <si>
-    <t>5,38</t>
-  </si>
-  <si>
-    <t>(-8.61281 41.1233)</t>
-  </si>
-  <si>
-    <t>A44 5+380C CVT743</t>
-  </si>
-  <si>
-    <t>A44 5+322D CVT746</t>
-  </si>
-  <si>
-    <t>(-8.61343 41.1231)</t>
-  </si>
-  <si>
-    <t>A44 5+322C CVT744</t>
-  </si>
-  <si>
-    <t>A44 5+165D CVT740</t>
-  </si>
-  <si>
-    <t>(-8.61517 41.1227)</t>
-  </si>
-  <si>
-    <t>A44 5+165C CVT739</t>
-  </si>
-  <si>
-    <t>A44 4+950D CV747</t>
-  </si>
-  <si>
-    <t>4,9</t>
-  </si>
-  <si>
-    <t>(-8.61807 41.1213)</t>
-  </si>
-  <si>
-    <t>A44 4+850D CV706</t>
-  </si>
-  <si>
-    <t>4,85</t>
-  </si>
-  <si>
-    <t>(-8.61919 41.1222)</t>
-  </si>
-  <si>
-    <t>A20 3+600D CV710</t>
-  </si>
-  <si>
-    <t>(-8.56823 41.1017)</t>
-  </si>
-  <si>
     <t>AEDL - A20 13+890 CT3711</t>
   </si>
   <si>
@@ -363,72 +267,15 @@
     <t>(-8.58972 41.1312)</t>
   </si>
   <si>
-    <t>A20 2+150D CV709</t>
-  </si>
-  <si>
-    <t>(-8.57493 41.0906)</t>
-  </si>
-  <si>
-    <t>A20 0+575C</t>
-  </si>
-  <si>
     <t>Carvalhos - Nó de S. Lourenço</t>
   </si>
   <si>
-    <t>0,5</t>
-  </si>
-  <si>
-    <t>(-8.57773 41.0765)</t>
-  </si>
-  <si>
-    <t>A1 300+450C CV715</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
     <t>A44/A29 - Canidelo</t>
   </si>
   <si>
-    <t>300,4</t>
-  </si>
-  <si>
-    <t>(-8.63574 41.1271)</t>
-  </si>
-  <si>
-    <t>A44 7+200C CV707</t>
-  </si>
-  <si>
-    <t>7,2</t>
-  </si>
-  <si>
-    <t>(-8.59403 41.1281)</t>
-  </si>
-  <si>
-    <t>A1 300+450C CF</t>
-  </si>
-  <si>
-    <t>A44 5+435D CVT741</t>
-  </si>
-  <si>
-    <t>A1 298+680D (Norte)</t>
-  </si>
-  <si>
-    <t>298,6</t>
-  </si>
-  <si>
-    <t>(-8.62526 41.1151)</t>
-  </si>
-  <si>
-    <t>A1 298+680D (Sul)</t>
-  </si>
-  <si>
-    <t>A1 298+680D (Este)</t>
-  </si>
-  <si>
-    <t>A1 298+680D (Oeste)</t>
-  </si>
-  <si>
     <t>AEDL - A20 0+650 CT3683</t>
   </si>
   <si>
@@ -438,18 +285,9 @@
     <t>(-8.57748 41.0773)</t>
   </si>
   <si>
-    <t>A1 297+150C CV713</t>
-  </si>
-  <si>
     <t>Santo Ovideo - A44/A29</t>
   </si>
   <si>
-    <t>297,1</t>
-  </si>
-  <si>
-    <t>(-8.6095 41.1115)</t>
-  </si>
-  <si>
     <t>AEDL - A1 297+975 CT3687</t>
   </si>
   <si>
@@ -520,24 +358,6 @@
   </si>
   <si>
     <t>(-8.58092 41.1437)</t>
-  </si>
-  <si>
-    <t>AEDL - A1 300+920C PM1209</t>
-  </si>
-  <si>
-    <t>AEDL - A1 300+920D PM1210</t>
-  </si>
-  <si>
-    <t>A1 302+460C CV716</t>
-  </si>
-  <si>
-    <t>A1 298+680D CV714</t>
-  </si>
-  <si>
-    <t>AEDL - A1 297+975C PM1208</t>
-  </si>
-  <si>
-    <t>Santo Ovídeo - Nó Coimbrões</t>
   </si>
   <si>
     <t>(long, lat)</t>
@@ -698,8 +518,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:G75" totalsRowShown="0">
-  <autoFilter ref="B1:G75" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}" name="Table1" displayName="Table1" ref="B1:G44" totalsRowShown="0">
+  <autoFilter ref="B1:G44" xr:uid="{EA5047B8-BA0E-4C00-9F73-78878BE13A40}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{DA4E266E-78B3-49ED-9193-E0A12C370FEF}" name="Network"/>
     <tableColumn id="1" xr3:uid="{405EBCE7-98B6-4D09-8211-78934C2737E1}" name="Equipamento"/>
@@ -1011,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F696A670-22A4-4677-8004-07E2A17F99A5}">
   <dimension ref="B1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +849,7 @@
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -1047,12 +867,12 @@
         <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>171</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1072,7 +892,7 @@
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1092,7 +912,7 @@
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -1112,7 +932,7 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -1132,7 +952,7 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -1153,7 +973,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
@@ -1173,7 +993,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -1194,7 +1014,7 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -1215,7 +1035,7 @@
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1235,7 +1055,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
         <v>42</v>
@@ -1256,7 +1076,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
@@ -1276,1148 +1096,542 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
         <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="G19" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="F20" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21">
-        <v>5.9749999999999996</v>
+        <v>77</v>
+      </c>
+      <c r="F21" t="s">
+        <v>78</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="F22" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C23" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="G23" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="E24" t="s">
-        <v>81</v>
-      </c>
-      <c r="F24">
-        <v>5.4349999999999996</v>
+        <v>82</v>
+      </c>
+      <c r="F24" t="s">
+        <v>91</v>
       </c>
       <c r="G24" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="F25" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="F26" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27">
-        <v>5.3220000000000001</v>
+        <v>98</v>
+      </c>
+      <c r="F27" t="s">
+        <v>99</v>
       </c>
       <c r="G27" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28">
-        <v>5.3220000000000001</v>
+        <v>36</v>
+      </c>
+      <c r="F28" t="s">
+        <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
-      </c>
-      <c r="F29">
-        <v>5.165</v>
+        <v>105</v>
+      </c>
+      <c r="F29" t="s">
+        <v>106</v>
       </c>
       <c r="G29" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>201</v>
+        <v>141</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>81</v>
-      </c>
-      <c r="F30">
-        <v>5.165</v>
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>109</v>
       </c>
       <c r="G30" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="G31" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" t="s">
-        <v>81</v>
-      </c>
-      <c r="F32" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="G32" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="G33" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" t="s">
-        <v>102</v>
-      </c>
-      <c r="F34" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="G34" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>81</v>
-      </c>
-      <c r="F35" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="G35" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C36" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>109</v>
-      </c>
-      <c r="F36" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="G36" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" t="s">
-        <v>54</v>
-      </c>
-      <c r="F37" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="G37" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
-      </c>
-      <c r="D38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" t="s">
-        <v>115</v>
-      </c>
-      <c r="F38" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="G38" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
-      </c>
-      <c r="D39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E39" t="s">
-        <v>120</v>
-      </c>
-      <c r="F39" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="G39" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C40" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" t="s">
-        <v>109</v>
-      </c>
-      <c r="F40" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G40" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C41" t="s">
-        <v>126</v>
-      </c>
-      <c r="D41" t="s">
-        <v>119</v>
-      </c>
-      <c r="E41" t="s">
-        <v>120</v>
-      </c>
-      <c r="F41" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="G41" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C42" t="s">
-        <v>127</v>
-      </c>
-      <c r="D42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
-        <v>81</v>
-      </c>
-      <c r="F42">
-        <v>5.4349999999999996</v>
+        <v>131</v>
       </c>
       <c r="G42" t="s">
-        <v>82</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>128</v>
-      </c>
-      <c r="D43" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" t="s">
-        <v>120</v>
-      </c>
-      <c r="F43" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G43" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>201</v>
+        <v>142</v>
       </c>
       <c r="C44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E44" t="s">
-        <v>120</v>
-      </c>
-      <c r="F44" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G44" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>201</v>
-      </c>
-      <c r="C45" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" t="s">
-        <v>120</v>
-      </c>
-      <c r="F45" t="s">
-        <v>129</v>
-      </c>
-      <c r="G45" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>201</v>
-      </c>
-      <c r="C46" t="s">
-        <v>133</v>
-      </c>
-      <c r="D46" t="s">
-        <v>119</v>
-      </c>
-      <c r="E46" t="s">
-        <v>120</v>
-      </c>
-      <c r="F46" t="s">
-        <v>129</v>
-      </c>
-      <c r="G46" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>201</v>
-      </c>
-      <c r="C47" t="s">
-        <v>134</v>
-      </c>
-      <c r="D47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" t="s">
-        <v>115</v>
-      </c>
-      <c r="F47" t="s">
-        <v>135</v>
-      </c>
-      <c r="G47" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>201</v>
-      </c>
-      <c r="C48" t="s">
-        <v>137</v>
-      </c>
-      <c r="D48" t="s">
-        <v>119</v>
-      </c>
-      <c r="E48" t="s">
-        <v>138</v>
-      </c>
-      <c r="F48" t="s">
         <v>139</v>
       </c>
-      <c r="G48" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>201</v>
-      </c>
-      <c r="C49" t="s">
-        <v>141</v>
-      </c>
-      <c r="D49" t="s">
-        <v>119</v>
-      </c>
-      <c r="E49" t="s">
-        <v>138</v>
-      </c>
-      <c r="F49" t="s">
-        <v>142</v>
-      </c>
-      <c r="G49" t="s">
-        <v>143</v>
-      </c>
+    </row>
+    <row r="49" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>201</v>
-      </c>
-      <c r="C50" t="s">
-        <v>144</v>
-      </c>
-      <c r="D50" t="s">
-        <v>119</v>
-      </c>
-      <c r="E50" t="s">
-        <v>120</v>
-      </c>
-      <c r="F50" t="s">
-        <v>145</v>
-      </c>
-      <c r="G50" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>201</v>
-      </c>
-      <c r="C51" t="s">
-        <v>147</v>
-      </c>
-      <c r="D51" t="s">
-        <v>119</v>
-      </c>
-      <c r="E51" t="s">
-        <v>148</v>
-      </c>
-      <c r="F51" t="s">
-        <v>149</v>
-      </c>
-      <c r="G51" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>201</v>
-      </c>
-      <c r="C52" t="s">
-        <v>151</v>
-      </c>
-      <c r="D52" t="s">
-        <v>119</v>
-      </c>
-      <c r="E52" t="s">
-        <v>152</v>
-      </c>
-      <c r="F52" t="s">
-        <v>153</v>
-      </c>
-      <c r="G52" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>201</v>
-      </c>
-      <c r="C53" t="s">
-        <v>155</v>
-      </c>
-      <c r="D53" t="s">
-        <v>119</v>
-      </c>
-      <c r="E53" t="s">
-        <v>152</v>
-      </c>
-      <c r="F53" t="s">
-        <v>153</v>
-      </c>
-      <c r="G53" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>201</v>
-      </c>
-      <c r="C54" t="s">
-        <v>157</v>
-      </c>
-      <c r="D54" t="s">
-        <v>35</v>
-      </c>
-      <c r="E54" t="s">
-        <v>36</v>
-      </c>
-      <c r="F54" t="s">
-        <v>40</v>
-      </c>
-      <c r="G54" t="s">
-        <v>41</v>
-      </c>
+    <row r="54" spans="9:12" x14ac:dyDescent="0.25">
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>201</v>
-      </c>
-      <c r="C55" t="s">
-        <v>158</v>
-      </c>
-      <c r="D55" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" t="s">
-        <v>159</v>
-      </c>
-      <c r="F55" t="s">
-        <v>160</v>
-      </c>
-      <c r="G55" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>201</v>
-      </c>
-      <c r="C56" t="s">
-        <v>162</v>
-      </c>
-      <c r="D56" t="s">
-        <v>10</v>
-      </c>
-      <c r="E56" t="s">
-        <v>11</v>
-      </c>
-      <c r="F56" t="s">
-        <v>163</v>
-      </c>
-      <c r="G56" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>201</v>
-      </c>
-      <c r="C57" t="s">
-        <v>165</v>
-      </c>
-      <c r="D57" t="s">
-        <v>119</v>
-      </c>
-      <c r="E57" t="s">
-        <v>148</v>
-      </c>
-      <c r="F57" t="s">
-        <v>149</v>
-      </c>
-      <c r="G57" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>201</v>
-      </c>
-      <c r="C58" t="s">
-        <v>166</v>
-      </c>
-      <c r="D58" t="s">
-        <v>119</v>
-      </c>
-      <c r="E58" t="s">
-        <v>148</v>
-      </c>
-      <c r="F58" t="s">
-        <v>149</v>
-      </c>
-      <c r="G58" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>201</v>
-      </c>
-      <c r="C59" t="s">
-        <v>167</v>
-      </c>
-      <c r="D59" t="s">
-        <v>119</v>
-      </c>
-      <c r="E59" t="s">
-        <v>152</v>
-      </c>
-      <c r="F59" t="s">
-        <v>153</v>
-      </c>
-      <c r="G59" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>201</v>
-      </c>
-      <c r="C60" t="s">
-        <v>168</v>
-      </c>
-      <c r="D60" t="s">
-        <v>119</v>
-      </c>
-      <c r="E60" t="s">
-        <v>120</v>
-      </c>
-      <c r="F60" t="s">
-        <v>129</v>
-      </c>
-      <c r="G60" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>201</v>
-      </c>
-      <c r="C61" t="s">
-        <v>169</v>
-      </c>
-      <c r="D61" t="s">
-        <v>119</v>
-      </c>
-      <c r="E61" t="s">
-        <v>170</v>
-      </c>
-      <c r="F61" t="s">
-        <v>142</v>
-      </c>
-      <c r="G61" t="s">
-        <v>143</v>
-      </c>
+    <row r="61" spans="9:12" x14ac:dyDescent="0.25">
       <c r="L61" s="1"/>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>202</v>
-      </c>
-      <c r="C62" t="s">
-        <v>172</v>
-      </c>
-      <c r="G62" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>202</v>
-      </c>
-      <c r="C63" t="s">
-        <v>173</v>
-      </c>
-      <c r="G63" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>202</v>
-      </c>
-      <c r="C64" t="s">
-        <v>174</v>
-      </c>
-      <c r="G64" t="s">
-        <v>178</v>
-      </c>
+    <row r="64" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>202</v>
-      </c>
-      <c r="C65" t="s">
-        <v>175</v>
-      </c>
-      <c r="G65" t="s">
-        <v>179</v>
-      </c>
+    <row r="65" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>202</v>
-      </c>
-      <c r="C66" t="s">
-        <v>180</v>
-      </c>
-      <c r="G66" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>202</v>
-      </c>
-      <c r="C67" t="s">
-        <v>181</v>
-      </c>
-      <c r="G67" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>202</v>
-      </c>
-      <c r="C68" t="s">
-        <v>182</v>
-      </c>
-      <c r="G68" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>202</v>
-      </c>
-      <c r="C69" t="s">
-        <v>183</v>
-      </c>
-      <c r="G69" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>202</v>
-      </c>
-      <c r="C70" t="s">
-        <v>188</v>
-      </c>
-      <c r="G70" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>202</v>
-      </c>
-      <c r="C71" t="s">
-        <v>189</v>
-      </c>
-      <c r="G71" t="s">
-        <v>195</v>
-      </c>
+    <row r="71" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>202</v>
-      </c>
-      <c r="C72" t="s">
-        <v>190</v>
-      </c>
-      <c r="G72" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>202</v>
-      </c>
-      <c r="C73" t="s">
-        <v>191</v>
-      </c>
-      <c r="G73" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>202</v>
-      </c>
-      <c r="C74" t="s">
-        <v>192</v>
-      </c>
-      <c r="G74" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>202</v>
-      </c>
-      <c r="C75" t="s">
-        <v>193</v>
-      </c>
-      <c r="G75" t="s">
-        <v>199</v>
-      </c>
+    <row r="75" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="9:10" x14ac:dyDescent="0.25">
       <c r="J76" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started running for VCI Nó de Coimbrões
</commit_message>
<xml_diff>
--- a/data/sensor_locations.xlsx
+++ b/data/sensor_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulinho\Desktop\Master-Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D68DE9D-0C31-4BE0-AB8D-62E0BF967DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1830F279-CF64-401A-B373-49CFE537F2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BD23C080-A3E8-4A95-931E-7578B8E55267}"/>
   </bookViews>
@@ -402,34 +402,34 @@
     <t>CAV401-2/CAV401-1_C</t>
   </si>
   <si>
-    <t>(-8.626663 41.112)</t>
-  </si>
-  <si>
-    <t>(-8.626322 41.112)</t>
-  </si>
-  <si>
     <t>AEDL - A1 297+975 CT3687_C</t>
   </si>
   <si>
     <t>AEDL - A1 297+975 CT3687_D</t>
   </si>
   <si>
-    <t>(-8.623002 41.114236)</t>
-  </si>
-  <si>
-    <t>(-8.622778 41.114559)</t>
-  </si>
-  <si>
     <t>AEDL - A1 300+250 CT3688_C</t>
   </si>
   <si>
     <t>AEDL - A1 300+250 CT3688_D</t>
   </si>
   <si>
-    <t>(-8.635923 41.120826)</t>
-  </si>
-  <si>
-    <t>(-8.635439 41.121116)</t>
+    <t>(-8.636215 41.123872)</t>
+  </si>
+  <si>
+    <t>(-8.635640 41.124475)</t>
+  </si>
+  <si>
+    <t>(-8.626214 41.110031)</t>
+  </si>
+  <si>
+    <t>(-8.626670 41.110078)</t>
+  </si>
+  <si>
+    <t>(-8.613747 41.112158)</t>
+  </si>
+  <si>
+    <t>(-8.615451 41.112901)</t>
   </si>
 </sst>
 </file>
@@ -811,7 +811,7 @@
   <dimension ref="B1:M76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +886,7 @@
         <v>3.6</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>3.6</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
@@ -1220,7 +1220,7 @@
         <v>116</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>64</v>
@@ -1232,7 +1232,7 @@
         <v>297.89999999999998</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
         <v>116</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>64</v>
@@ -1252,7 +1252,7 @@
         <v>297.89999999999998</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
@@ -1260,7 +1260,7 @@
         <v>116</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>64</v>
@@ -1272,7 +1272,7 @@
         <v>300.2</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
@@ -1280,7 +1280,7 @@
         <v>116</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>64</v>
@@ -1292,7 +1292,7 @@
         <v>300.2</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>